<commit_message>
Create HumanMessage with content from "Templates" sheet.
</commit_message>
<xml_diff>
--- a/mapping_spec/Mapping Specification.xlsx
+++ b/mapping_spec/Mapping Specification.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\PycharmProjects\XSLTMapper\mapping_spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D0B4BA-32B5-4A9A-BD0A-808452F3ED68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC38CE45-AA50-4CDF-9399-29F50DCCE82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26760" yWindow="8625" windowWidth="51360" windowHeight="23445" activeTab="1" xr2:uid="{702BBFDF-DA53-46B0-8260-7E02A283EC47}"/>
+    <workbookView xWindow="3165" yWindow="5625" windowWidth="51360" windowHeight="23445" xr2:uid="{702BBFDF-DA53-46B0-8260-7E02A283EC47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapping Specification" sheetId="1" r:id="rId1"/>
+    <sheet name="Mappings" sheetId="1" r:id="rId1"/>
     <sheet name="Templates" sheetId="4" r:id="rId2"/>
     <sheet name="System Prompt" sheetId="2" r:id="rId3"/>
     <sheet name="User Prompt" sheetId="3" r:id="rId4"/>
@@ -1260,10 +1260,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1604,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC0D92E-1B46-46D9-BF78-D7203D450837}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D68AC26-A9AF-43AE-B0A1-AA3A5EE88B76}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>